<commit_message>
updated template and example files
</commit_message>
<xml_diff>
--- a/stability_stats_example.xlsx
+++ b/stability_stats_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10294643\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10294643\Documents\R\stability-regression-app-2\stability-regression-shiny-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDA0877-9B01-4739-9B81-30EC68AA465B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151CFA6E-E1AC-4EFA-A512-4DF3E7F1C975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC9638E3-476B-4822-ACD0-A879084F2FD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC9638E3-476B-4822-ACD0-A879084F2FD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>HuNHP CD3 (SP34-2) R718</t>
   </si>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t>Specimen_002_H7_H07.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_A8_A08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_B8_B08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_C8_C08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_D8_D08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_E8_E08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_F8_F08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_G8_G08.fcs</t>
+  </si>
+  <si>
+    <t>Specimen_002_H8_H08.fcs</t>
   </si>
 </sst>
 </file>
@@ -231,7 +255,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,12 +277,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFC9388"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -321,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,10 +361,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,15 +688,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6436E6-23E2-47F2-8682-104E57A49C18}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:G57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -708,7 +733,7 @@
       <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="12">
         <v>30</v>
       </c>
       <c r="D2" s="5">
@@ -731,7 +756,7 @@
       <c r="B3" s="8">
         <v>0.5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>30</v>
       </c>
       <c r="D3" s="5">
@@ -754,7 +779,7 @@
       <c r="B4" s="8">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="12">
         <v>30</v>
       </c>
       <c r="D4" s="5">
@@ -777,7 +802,7 @@
       <c r="B5" s="8">
         <v>1.5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>30</v>
       </c>
       <c r="D5" s="5">
@@ -800,7 +825,7 @@
       <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>30</v>
       </c>
       <c r="D6" s="5">
@@ -823,7 +848,7 @@
       <c r="B7" s="8">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <v>30</v>
       </c>
       <c r="D7" s="5">
@@ -846,7 +871,7 @@
       <c r="B8" s="8">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <v>30</v>
       </c>
       <c r="D8" s="5">
@@ -869,7 +894,7 @@
       <c r="B9" s="8">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <v>30</v>
       </c>
       <c r="D9" s="5">
@@ -892,7 +917,7 @@
       <c r="B10" s="5">
         <v>0</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <v>60</v>
       </c>
       <c r="D10" s="6">
@@ -915,7 +940,7 @@
       <c r="B11" s="5">
         <v>0.5</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <v>60</v>
       </c>
       <c r="D11" s="6">
@@ -938,7 +963,7 @@
       <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <v>60</v>
       </c>
       <c r="D12" s="6">
@@ -961,7 +986,7 @@
       <c r="B13" s="5">
         <v>1.5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="12">
         <v>60</v>
       </c>
       <c r="D13" s="6">
@@ -984,7 +1009,7 @@
       <c r="B14" s="5">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="12">
         <v>60</v>
       </c>
       <c r="D14" s="6">
@@ -1007,7 +1032,7 @@
       <c r="B15" s="5">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="12">
         <v>60</v>
       </c>
       <c r="D15" s="6">
@@ -1030,7 +1055,7 @@
       <c r="B16" s="5">
         <v>4</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="12">
         <v>60</v>
       </c>
       <c r="D16" s="6">
@@ -1053,7 +1078,7 @@
       <c r="B17" s="5">
         <v>5</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="12">
         <v>60</v>
       </c>
       <c r="D17" s="6">
@@ -1076,7 +1101,7 @@
       <c r="B18" s="5">
         <v>0</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="12">
         <v>125</v>
       </c>
       <c r="D18" s="5">
@@ -1099,7 +1124,7 @@
       <c r="B19" s="5">
         <v>0.5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="12">
         <v>125</v>
       </c>
       <c r="D19" s="5">
@@ -1122,7 +1147,7 @@
       <c r="B20" s="5">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="12">
         <v>125</v>
       </c>
       <c r="D20" s="5">
@@ -1145,7 +1170,7 @@
       <c r="B21" s="5">
         <v>1.5</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>125</v>
       </c>
       <c r="D21" s="5">
@@ -1168,7 +1193,7 @@
       <c r="B22" s="5">
         <v>2</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="12">
         <v>125</v>
       </c>
       <c r="D22" s="5">
@@ -1191,7 +1216,7 @@
       <c r="B23" s="5">
         <v>3</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12">
         <v>125</v>
       </c>
       <c r="D23" s="5">
@@ -1214,7 +1239,7 @@
       <c r="B24" s="5">
         <v>4</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12">
         <v>125</v>
       </c>
       <c r="D24" s="5">
@@ -1237,7 +1262,7 @@
       <c r="B25" s="5">
         <v>5</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="12">
         <v>125</v>
       </c>
       <c r="D25" s="5">
@@ -1260,7 +1285,7 @@
       <c r="B26" s="5">
         <v>0</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="12">
         <v>250</v>
       </c>
       <c r="D26" s="6">
@@ -1283,7 +1308,7 @@
       <c r="B27" s="5">
         <v>0.5</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="12">
         <v>250</v>
       </c>
       <c r="D27" s="6">
@@ -1306,7 +1331,7 @@
       <c r="B28" s="5">
         <v>1</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="12">
         <v>250</v>
       </c>
       <c r="D28" s="6">
@@ -1329,7 +1354,7 @@
       <c r="B29" s="5">
         <v>1.5</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="12">
         <v>250</v>
       </c>
       <c r="D29" s="6">
@@ -1352,7 +1377,7 @@
       <c r="B30" s="5">
         <v>2</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="12">
         <v>250</v>
       </c>
       <c r="D30" s="6">
@@ -1375,7 +1400,7 @@
       <c r="B31" s="5">
         <v>3</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="12">
         <v>250</v>
       </c>
       <c r="D31" s="6">
@@ -1398,7 +1423,7 @@
       <c r="B32" s="5">
         <v>4</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="12">
         <v>250</v>
       </c>
       <c r="D32" s="6">
@@ -1421,7 +1446,7 @@
       <c r="B33" s="5">
         <v>5</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="12">
         <v>250</v>
       </c>
       <c r="D33" s="6">
@@ -1444,7 +1469,7 @@
       <c r="B34" s="5">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="12">
         <v>500</v>
       </c>
       <c r="D34" s="5">
@@ -1467,7 +1492,7 @@
       <c r="B35" s="5">
         <v>0.5</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="12">
         <v>500</v>
       </c>
       <c r="D35" s="5">
@@ -1490,7 +1515,7 @@
       <c r="B36" s="5">
         <v>1</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="12">
         <v>500</v>
       </c>
       <c r="D36" s="5">
@@ -1513,7 +1538,7 @@
       <c r="B37" s="5">
         <v>1.5</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="12">
         <v>500</v>
       </c>
       <c r="D37" s="5">
@@ -1536,7 +1561,7 @@
       <c r="B38" s="5">
         <v>2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="12">
         <v>500</v>
       </c>
       <c r="D38" s="5">
@@ -1559,7 +1584,7 @@
       <c r="B39" s="5">
         <v>3</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="12">
         <v>500</v>
       </c>
       <c r="D39" s="5">
@@ -1582,7 +1607,7 @@
       <c r="B40" s="5">
         <v>4</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="12">
         <v>500</v>
       </c>
       <c r="D40" s="5">
@@ -1605,7 +1630,7 @@
       <c r="B41" s="5">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="12">
         <v>500</v>
       </c>
       <c r="D41" s="5">
@@ -1628,7 +1653,7 @@
       <c r="B42" s="5">
         <v>0</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="12">
         <v>1000</v>
       </c>
       <c r="D42" s="6">
@@ -1651,7 +1676,7 @@
       <c r="B43" s="5">
         <v>0.5</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="12">
         <v>1000</v>
       </c>
       <c r="D43" s="6">
@@ -1674,7 +1699,7 @@
       <c r="B44" s="5">
         <v>1</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="12">
         <v>1000</v>
       </c>
       <c r="D44" s="6">
@@ -1697,7 +1722,7 @@
       <c r="B45" s="5">
         <v>1.5</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="12">
         <v>1000</v>
       </c>
       <c r="D45" s="6">
@@ -1720,7 +1745,7 @@
       <c r="B46" s="5">
         <v>2</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="12">
         <v>1000</v>
       </c>
       <c r="D46" s="6">
@@ -1743,7 +1768,7 @@
       <c r="B47" s="5">
         <v>3</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="12">
         <v>1000</v>
       </c>
       <c r="D47" s="6">
@@ -1766,7 +1791,7 @@
       <c r="B48" s="5">
         <v>4</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="12">
         <v>1000</v>
       </c>
       <c r="D48" s="6">
@@ -1789,7 +1814,7 @@
       <c r="B49" s="5">
         <v>5</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="12">
         <v>1000</v>
       </c>
       <c r="D49" s="6">
@@ -1806,8 +1831,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>54</v>
+      <c r="A50" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B50" s="5">
         <v>0</v>
@@ -1829,8 +1854,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>54</v>
+      <c r="A51" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B51" s="5">
         <v>0.5</v>
@@ -1852,8 +1877,8 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>54</v>
+      <c r="A52" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -1875,8 +1900,8 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>54</v>
+      <c r="A53" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="B53" s="5">
         <v>1.5</v>
@@ -1898,8 +1923,8 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>54</v>
+      <c r="A54" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B54" s="5">
         <v>2</v>
@@ -1921,8 +1946,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>54</v>
+      <c r="A55" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="B55" s="5">
         <v>3</v>
@@ -1944,8 +1969,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>54</v>
+      <c r="A56" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B56" s="5">
         <v>4</v>
@@ -1967,8 +1992,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>54</v>
+      <c r="A57" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="B57" s="5">
         <v>5</v>
@@ -1990,32 +2015,56 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="10"/>
     </row>
     <row r="59" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="10"/>
     </row>
     <row r="60" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="10"/>
     </row>
     <row r="61" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D62" s="9"/>
-      <c r="E62" s="9"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G57">

</xml_diff>

<commit_message>
updated stability example template header
</commit_message>
<xml_diff>
--- a/stability_stats_example.xlsx
+++ b/stability_stats_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10294643\Documents\R\stability-regression-app-2\stability-regression-shiny-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151CFA6E-E1AC-4EFA-A512-4DF3E7F1C975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7192343A-F5B7-4296-93FB-624CBB8B185B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC9638E3-476B-4822-ACD0-A879084F2FD9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AC9638E3-476B-4822-ACD0-A879084F2FD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
-    <t>HuNHP CD3 (SP34-2) R718</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Specimen_002_H8_H08.fcs</t>
+  </si>
+  <si>
+    <t>Filenames</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -705,30 +705,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="8">
         <v>0.5</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8">
         <v>1</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8">
         <v>1.5</v>
@@ -820,7 +820,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="8">
         <v>4</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8">
         <v>5</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>0</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5">
         <v>0.5</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5">
         <v>1.5</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5">
         <v>3</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5">
         <v>4</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5">
         <v>5</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="5">
         <v>0</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="5">
         <v>0.5</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="5">
         <v>1.5</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="5">
         <v>2</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="5">
         <v>3</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="5">
         <v>4</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" s="5">
         <v>5</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5">
         <v>0</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="5">
         <v>0.5</v>
@@ -1326,7 +1326,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -1349,7 +1349,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="5">
         <v>1.5</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="5">
         <v>2</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="5">
         <v>3</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="5">
         <v>4</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="5">
         <v>5</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="5">
         <v>0</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="5">
         <v>0.5</v>
@@ -1510,7 +1510,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="5">
         <v>1.5</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="5">
         <v>2</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="5">
         <v>3</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="5">
         <v>4</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="5">
         <v>5</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="5">
         <v>0.5</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="5">
         <v>1.5</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="5">
         <v>2</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="5">
         <v>3</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="5">
         <v>4</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="5">
         <v>5</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="5">
         <v>0</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="5">
         <v>0.5</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="5">
         <v>1.5</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="5">
         <v>2</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B55" s="5">
         <v>3</v>
@@ -1970,7 +1970,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B56" s="5">
         <v>4</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="57" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="5">
         <v>5</v>

</xml_diff>